<commit_message>
Regeln für Artikelbezug ergänzt
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/Formular_Projektsonderabrechnung_Simple.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/Formular_Projektsonderabrechnung_Simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sxDaten\GitHub\DataFactory-Knowledge-Center\8. Harmonising standards\01_Project organisation\03_Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217299BE-EEBD-4A34-B4BA-49390A29B513}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC59DA1-83BF-4CCA-A02A-A83429F233B3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{59CE7F71-93D6-4922-87C0-A5C407BF9C6A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>PLAN</t>
   </si>
@@ -732,16 +732,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>486834</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3307292</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>89956</xdr:rowOff>
+      <xdr:rowOff>179914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>635001</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>693207</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -756,8 +756,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7175501" y="4153956"/>
-          <a:ext cx="7239000" cy="1756835"/>
+          <a:off x="5032375" y="4243914"/>
+          <a:ext cx="8731249" cy="1989669"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -813,6 +813,32 @@
               </a:solidFill>
             </a:rPr>
             <a:t> Abrechung folgt der Gliederung des Releaseplanes !</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Jede Leistungsposition muss eindeutig nur Datenintegration, DataFactory oder Sonstiges umfassen -  um den korrekten MyF Artikel anzusprechen.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Dem MyF Angebot wird der Releaseplan beigefügt als Anlage -  das Angebot differenziert nur Datenintegration, DataFactory, Sonstiges, Reisekosten</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1269,7 +1295,7 @@
   <dimension ref="A1:CM57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3354,7 +3380,7 @@
     <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A52" s="7"/>
       <c r="D52" s="13">
-        <f t="shared" ref="D52:R52" si="13">SUM(D15:D51)</f>
+        <f t="shared" ref="D52:E52" si="13">SUM(D15:D51)</f>
         <v>0</v>
       </c>
       <c r="E52" s="13">

</xml_diff>